<commit_message>
Added Create aggregation Task and Debug Scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/DataFiles/loginData.xlsx
+++ b/src/test/resources/DataFiles/loginData.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="2" r:id="rId1"/>
     <sheet name="JDBCAPPLICATION" sheetId="3" r:id="rId2"/>
+    <sheet name="IdentityMappings" sheetId="4" r:id="rId3"/>
+    <sheet name="DeBugOperations" sheetId="5" r:id="rId4"/>
+    <sheet name="CreateAggregationTask" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -135,6 +138,48 @@
   <si>
     <t>firstname</t>
   </si>
+  <si>
+    <t>IdentityMappingName</t>
+  </si>
+  <si>
+    <t>AttributeName</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>SelectAnObject</t>
+  </si>
+  <si>
+    <t>SearchByNameOrID</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>AggregationTaskName</t>
+  </si>
+  <si>
+    <t>ApplicationAggregationType</t>
+  </si>
+  <si>
+    <t>EmployeeAgg</t>
+  </si>
+  <si>
+    <t>AccountAggregartion</t>
+  </si>
 </sst>
 </file>
 
@@ -146,7 +191,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +206,19 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF0000C0"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -312,12 +370,6 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF2A00FF"/>
-      <name val="Courier New"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -653,142 +705,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,13 +1163,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="26.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="22.4285714285714" customWidth="1"/>
@@ -1129,26 +1184,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1163,8 +1202,8 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1210,32 +1249,175 @@
       </c>
     </row>
     <row r="2" spans="1:9">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="26.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="30.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="36.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="25.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="30.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="29.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="35.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="33.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="40.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>